<commit_message>
tidy data final ;)
</commit_message>
<xml_diff>
--- a/_posts/2022-04-22-tidydata/messy_data.xlsx
+++ b/_posts/2022-04-22-tidydata/messy_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zablotski/Library/Mobile Documents/com~apple~CloudDocs/7. Hobby/programming and stats/yuzaR-Blog/_posts/2022-04-22-tidydata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649DFEB7-ACED-3E43-BE2A-29132B57CF8E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D860661D-F785-9C4E-8614-97070A199FE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="4" xr2:uid="{73549361-0994-4943-B6B3-BCBFC2B427CC}"/>
   </bookViews>
@@ -18,12 +18,13 @@
     <sheet name="2021" sheetId="3" r:id="rId3"/>
     <sheet name="tidy data" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2020'!$B$3:$H$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2020'!$A$1:$G$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'messy data '!$A$1:$E$4</definedName>
   </definedNames>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="52">
   <si>
     <t>Monday</t>
   </si>
@@ -53,15 +54,6 @@
     <t xml:space="preserve">      cat</t>
   </si>
   <si>
-    <t>comments</t>
-  </si>
-  <si>
-    <t>blah</t>
-  </si>
-  <si>
-    <t>go grocery shopping</t>
-  </si>
-  <si>
     <t>GROUP</t>
   </si>
   <si>
@@ -83,27 +75,15 @@
     <t>MISSING</t>
   </si>
   <si>
-    <t>I HATE STATISTICS!!! 🤬🤬🤬</t>
-  </si>
-  <si>
     <t>&lt; 38,2</t>
   </si>
   <si>
-    <t>SEX</t>
-  </si>
-  <si>
     <t>jaguar</t>
   </si>
   <si>
     <t>humanoid robot</t>
   </si>
   <si>
-    <t>DAYS IN A GLORIOUS LIFE OF ZOMBIES</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
     <t xml:space="preserve">cat.     </t>
   </si>
   <si>
@@ -116,9 +96,6 @@
     <t>CONTROLL</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>38.3 %</t>
   </si>
   <si>
@@ -128,9 +105,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>not needed column</t>
-  </si>
-  <si>
     <t>38,7 - 45,9</t>
   </si>
   <si>
@@ -155,9 +129,6 @@
     <t>c …</t>
   </si>
   <si>
-    <t>5 -&gt;8 (nach 1,5 Min)</t>
-  </si>
-  <si>
     <t>5 -&gt; 8 (after 1,5 min)</t>
   </si>
   <si>
@@ -198,6 +169,27 @@
   </si>
   <si>
     <t>female</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>2/3</t>
+  </si>
+  <si>
+    <t>0 - 5</t>
+  </si>
+  <si>
+    <t>&gt; 99</t>
+  </si>
+  <si>
+    <t>&lt; 3</t>
   </si>
 </sst>
 </file>
@@ -207,7 +199,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -240,20 +232,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,12 +247,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -291,7 +269,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -335,17 +313,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -463,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -481,9 +448,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -491,127 +455,100 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="justify"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1012,7 +949,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="251" workbookViewId="0">
-      <selection activeCell="B4" sqref="A1:E5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1026,28 +963,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="40" t="s">
+      <c r="A1" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="34" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D2" s="5">
         <v>150</v>
@@ -1058,10 +995,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C3" s="5">
         <v>13547</v>
@@ -1075,10 +1012,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C4" s="5">
         <v>0</v>
@@ -1092,10 +1029,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C5" s="5">
         <v>2561</v>
@@ -1114,477 +1051,352 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2682A8DF-FA49-A44E-9600-193C97BBC219}">
-  <dimension ref="B1:J20"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="5" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="6"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="E1" s="52" t="s">
+    <row r="1" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="35">
+        <v>1</v>
+      </c>
+      <c r="E1" s="35">
+        <v>2</v>
+      </c>
+      <c r="F1" s="36">
+        <v>3</v>
+      </c>
+      <c r="G1" s="37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="E2" s="1">
+        <v>38.5</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1">
+        <v>39.1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="8">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-    </row>
-    <row r="2" spans="2:10" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-    </row>
-    <row r="3" spans="2:10" ht="68" x14ac:dyDescent="0.2">
-      <c r="B3" s="10" t="s">
+      <c r="E4" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="7">
+        <v>38.6</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="41">
-        <v>1</v>
-      </c>
-      <c r="F3" s="41">
-        <v>2</v>
-      </c>
-      <c r="G3" s="42">
-        <v>3</v>
-      </c>
-      <c r="H3" s="43">
-        <v>4</v>
-      </c>
-      <c r="I3" s="7"/>
-      <c r="J3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>38.299999999999997</v>
-      </c>
-      <c r="F4" s="1">
-        <v>38.5</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="F5" s="1">
         <v>39.1</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="15">
+        <v>39.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="2">
+        <v>38.9</v>
+      </c>
+      <c r="F6" s="2">
+        <v>38.4</v>
+      </c>
+      <c r="G6" s="17">
+        <v>38.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="20">
+        <v>0</v>
+      </c>
+      <c r="D7" s="21">
         <v>38.299999999999997</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="J5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="29" t="s">
+      <c r="E7" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="21">
+        <v>38.4</v>
+      </c>
+      <c r="G7" s="22">
+        <v>39.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="9">
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="E8" s="1">
+        <v>38.5</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="25">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="E9" s="1">
+        <v>39.1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="25">
+        <v>38.4</v>
+      </c>
+      <c r="E10" s="1">
+        <v>38.4</v>
+      </c>
+      <c r="F10" s="1">
+        <v>38.6</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3">
         <v>2</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="D11" s="1">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="E11" s="1">
+        <v>39.9</v>
+      </c>
+      <c r="F11" s="1">
+        <v>39.1</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="8">
-        <v>38.6</v>
-      </c>
-      <c r="H6" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="1">
-        <v>39.1</v>
-      </c>
-      <c r="H7" s="16">
-        <v>39.9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="B8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="B12" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="27">
+        <v>1</v>
+      </c>
+      <c r="D12" s="28">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="E12" s="28">
         <v>38.9</v>
       </c>
-      <c r="G8" s="2">
+      <c r="F12" s="28">
         <v>38.4</v>
       </c>
-      <c r="H8" s="18">
+      <c r="G12" s="29">
         <v>38.9</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="21">
-        <v>0</v>
-      </c>
-      <c r="E9" s="22">
+    <row r="13" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="31">
+        <v>1</v>
+      </c>
+      <c r="D13" s="32">
         <v>38.299999999999997</v>
       </c>
-      <c r="F9" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="22">
+      <c r="E13" s="32">
+        <v>39.5</v>
+      </c>
+      <c r="F13" s="32">
         <v>38.4</v>
       </c>
-      <c r="H9" s="23">
+      <c r="G13" s="33">
         <v>39.5</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E11" s="49" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="51"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="41">
-        <v>1</v>
-      </c>
-      <c r="F12" s="41">
-        <v>2</v>
-      </c>
-      <c r="G12" s="42">
-        <v>3</v>
-      </c>
-      <c r="H12" s="43">
-        <v>4</v>
-      </c>
-      <c r="I12" s="7"/>
-      <c r="J12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="3">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1">
-        <v>38.299999999999997</v>
-      </c>
-      <c r="F13" s="1">
-        <v>38.5</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="26">
-        <v>22.482140000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="3">
-        <v>1</v>
-      </c>
-      <c r="E14" s="31">
-        <v>38.200000000000003</v>
-      </c>
-      <c r="F14" s="1">
-        <v>39.1</v>
-      </c>
-      <c r="G14" s="1">
-        <v>38.299999999999997</v>
-      </c>
-      <c r="H14" s="14"/>
-      <c r="J14" s="26">
-        <v>22.914290000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="3">
-        <v>1</v>
-      </c>
-      <c r="E15" s="31">
-        <v>38.4</v>
-      </c>
-      <c r="F15" s="1">
-        <v>38.4</v>
-      </c>
-      <c r="G15" s="1">
-        <v>38.6</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="J15" s="26">
-        <v>23.16667</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="3">
-        <v>2</v>
-      </c>
-      <c r="E16" s="1">
-        <v>38.200000000000003</v>
-      </c>
-      <c r="F16" s="1">
-        <v>39.9</v>
-      </c>
-      <c r="G16" s="1">
-        <v>39.1</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="J16" s="44" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B17" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="33">
-        <v>1</v>
-      </c>
-      <c r="E17" s="34">
-        <v>38.700000000000003</v>
-      </c>
-      <c r="F17" s="34">
-        <v>38.9</v>
-      </c>
-      <c r="G17" s="34">
-        <v>38.4</v>
-      </c>
-      <c r="H17" s="35">
-        <v>38.9</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="37">
-        <v>1</v>
-      </c>
-      <c r="E18" s="38">
-        <v>38.299999999999997</v>
-      </c>
-      <c r="F18" s="38">
-        <v>39.5</v>
-      </c>
-      <c r="G18" s="38">
-        <v>38.4</v>
-      </c>
-      <c r="H18" s="39">
-        <v>39.5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D19" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="25">
-        <f>SUM(E15:E18)</f>
-        <v>153.6</v>
-      </c>
-      <c r="F19" s="25">
-        <f t="shared" ref="F19:H19" si="0">SUM(F15:F18)</f>
-        <v>156.69999999999999</v>
-      </c>
-      <c r="G19" s="25">
-        <f t="shared" si="0"/>
-        <v>154.5</v>
-      </c>
-      <c r="H19" s="25">
-        <f t="shared" si="0"/>
-        <v>78.400000000000006</v>
-      </c>
-      <c r="I19"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D20" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="28">
-        <f>E19/4</f>
-        <v>38.4</v>
-      </c>
-      <c r="F20" s="28">
-        <f>F19*100/E19</f>
-        <v>102.01822916666666</v>
-      </c>
-      <c r="G20" s="28">
-        <f>G19*100/E19</f>
-        <v>100.5859375</v>
-      </c>
-      <c r="H20" s="28">
-        <f>H19*100/E19</f>
-        <v>51.041666666666671</v>
-      </c>
-      <c r="I20"/>
-    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="E1:H2"/>
-  </mergeCells>
-  <conditionalFormatting sqref="E4:G7">
+  <conditionalFormatting sqref="D2:F5">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
       <formula>39</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8:G8 E9 G9">
+  <conditionalFormatting sqref="D6:F6 D7 F7">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
       <formula>39</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
+  <conditionalFormatting sqref="G5">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
       <formula>39</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:H9">
+  <conditionalFormatting sqref="G6:G7">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
       <formula>39</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13:G16">
+  <conditionalFormatting sqref="D8:F11">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>39</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17:G18">
+  <conditionalFormatting sqref="D12:F13">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>39</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H16">
+  <conditionalFormatting sqref="G11">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>39</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H17:H18">
+  <conditionalFormatting sqref="G12:G13">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>39</formula>
     </cfRule>
@@ -1595,12 +1407,113 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2319F367-3662-0F49-9F69-B1D13ADC7B8B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="400" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1610,117 +1523,117 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="341" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="48" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="48" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="48" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="48" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="48" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7.83203125" style="48" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="48" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="48"/>
+    <col min="1" max="1" width="9.6640625" style="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="41" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="41" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="41" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.83203125" style="41" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="41" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="41"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="47"/>
+      <c r="A1" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47">
+      <c r="A2" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40">
         <v>13547</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="47" t="s">
+      <c r="A3" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="40">
         <v>150</v>
       </c>
-      <c r="D3" s="47">
+      <c r="D3" s="40">
         <v>977859</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="47" t="s">
+      <c r="A4" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="47">
+      <c r="C4" s="40">
         <v>140</v>
       </c>
-      <c r="D4" s="47">
-        <v>0</v>
-      </c>
-      <c r="E4" s="47"/>
+      <c r="D4" s="40">
+        <v>0</v>
+      </c>
+      <c r="E4" s="40"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="47">
-        <v>0</v>
-      </c>
-      <c r="D5" s="47">
+      <c r="A5" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="40">
+        <v>0</v>
+      </c>
+      <c r="D5" s="40">
         <v>2561</v>
       </c>
-      <c r="E5" s="47"/>
+      <c r="E5" s="40"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="47" t="s">
+      <c r="A6" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="47">
+      <c r="C6" s="40">
         <v>190</v>
       </c>
-      <c r="D6" s="47">
+      <c r="D6" s="40">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="47" t="s">
+      <c r="A7" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="47">
+      <c r="C7" s="40">
         <v>160</v>
       </c>
-      <c r="D7" s="47">
+      <c r="D7" s="40">
         <v>0</v>
       </c>
     </row>
@@ -1734,64 +1647,65 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="394" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="9" style="5"/>
+    <col min="1" max="1" width="9" style="43"/>
+    <col min="2" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>52</v>
+      <c r="A1" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
-        <v>23</v>
+      <c r="A2" s="43" t="s">
+        <v>49</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C2" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
-        <v>9</v>
+      <c r="A3" s="43" t="s">
+        <v>48</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
-        <v>37</v>
+      <c r="A4" s="43" t="s">
+        <v>51</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C4" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
-        <v>44</v>
+      <c r="A5" s="43" t="s">
+        <v>50</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
@@ -1800,4 +1714,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{460368D3-7C60-5445-BF02-65AF3189A82A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>